<commit_message>
Eccentric Tech - Defense Grid 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Aelanna/Eccentric Tech - Defense Grid - 3066838686/3066838686.xlsx
+++ b/Data/Aelanna/Eccentric Tech - Defense Grid - 3066838686/3066838686.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\Eccentric Tech - Defense Grid - 3066838686\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\1.4\Aelanna\Eccentric\Eccentric Tech - Defense Grid - 3066838686\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9142EBBE-0E19-4DF7-B4EC-76C4FED561E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9AEE9A-AC0F-469C-AF59-40A84D5388BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="788">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -2155,6 +2155,264 @@
   </si>
   <si>
     <t>ThingDef+Eccentric_ArtilleryDesignator.comps.2.verb.label</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ProjectorEffects</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ProjectorEffectsDesc</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ShowProjectorEffectsSelected</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ShowProjectorEffectsSelectedDesc</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ShowProjectorEffectsSelectedNetwork</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ShowProjectorEffectsSelectedNetworkDesc</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ShowProjectorEffectsDanger</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ShowProjectorEffectsDangerDesc</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ShieldRadiusLabel</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ShieldRadiusDesc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_Color</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ColorDesc</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ColorDefault</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ColorRedLabel</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ColorGreenLabel</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ColorBlueLabel</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ColorAlphaLabel</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ColorCopy</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ColorCopyDesc</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ColorPaste</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ColorPasteDesc</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ColorClear</t>
+  </si>
+  <si>
+    <t>EccentricDefenseGrid_ColorClearDesc</t>
+  </si>
+  <si>
+    <t>Shield Projector Effects</t>
+  </si>
+  <si>
+    <t>Determines when the shield projector field range overlays are visible. Note that shield systems are always active regardless even if they are not visible.</t>
+  </si>
+  <si>
+    <t>Show When Selected</t>
+  </si>
+  <si>
+    <t>Shows shield projector field overlays for selected projectors.</t>
+  </si>
+  <si>
+    <t>Show When Network Selected</t>
+  </si>
+  <si>
+    <t>Shows shield projector field overlays when any buildings in the same network are selected.</t>
+  </si>
+  <si>
+    <t>Show When In Danger</t>
+  </si>
+  <si>
+    <t>Shows shield projector field overlays when story danger is present on the current map.</t>
+  </si>
+  <si>
+    <t>Radius: {0}</t>
+  </si>
+  <si>
+    <t>Adjust the interception radius of this projector.</t>
+  </si>
+  <si>
+    <t>Change Color</t>
+  </si>
+  <si>
+    <t>Changes the color of this building. This change is purely visual and does not affect its functionality.</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>R: {0}</t>
+  </si>
+  <si>
+    <t>G: {0}</t>
+  </si>
+  <si>
+    <t>B: {0}</t>
+  </si>
+  <si>
+    <t>A: {0}</t>
+  </si>
+  <si>
+    <t>Copy Color</t>
+  </si>
+  <si>
+    <t>Copy the color of this building so it can be pasted to other buildings.</t>
+  </si>
+  <si>
+    <t>Paste Color</t>
+  </si>
+  <si>
+    <t>Paste the currently copied color onto this building.</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>Clear the copied color from the clipboard.</t>
+  </si>
+  <si>
+    <t>쉴드 프로젝터 효과</t>
+  </si>
+  <si>
+    <t>쉴드 프로젝터 필드 범위 오버레이가 표시되는 시기를 결정합니다. 쉴드 시스템은 보이지 않더라도 항상 활성화되어 있다는 점에 유의하세요.</t>
+  </si>
+  <si>
+    <t>선택 시 표시</t>
+  </si>
+  <si>
+    <t>선택한 프로젝터에 대한 쉴드 프로젝터 필드 오버레이를 표시합니다.</t>
+  </si>
+  <si>
+    <t>네트워크 선택 시 표시</t>
+  </si>
+  <si>
+    <t>같은 네트워크에 있는 건물이 선택되면 쉴드 프로젝터 필드 오버레이를 표시합니다.</t>
+  </si>
+  <si>
+    <t>위험에 처했을 때 표시</t>
+  </si>
+  <si>
+    <t>현재 맵에 스토리 위험이 존재할 때 쉴드 프로젝터 필드 오버레이를 표시합니다.</t>
+  </si>
+  <si>
+    <t>반경: {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 프로젝터의 차단 반경을 조정합니다.</t>
+  </si>
+  <si>
+    <t>색상 변경</t>
+  </si>
+  <si>
+    <t>이 건물의 색상을 변경합니다. 이 변경은 순전히 시각적인 효과이며 기능에는 영향을 미치지 않습니다.</t>
+  </si>
+  <si>
+    <t>기본값</t>
+  </si>
+  <si>
+    <t>색상 복사</t>
+  </si>
+  <si>
+    <t>이 건물의 색상을 복사하여 다른 건물에 붙여넣을 수 있습니다.</t>
+  </si>
+  <si>
+    <t>색상 붙여넣기</t>
+  </si>
+  <si>
+    <t>현재 복사한 색상을 이 건물에 붙여넣습니다.</t>
+  </si>
+  <si>
+    <t>지우기</t>
+  </si>
+  <si>
+    <t>클립보드에서 복사한 색상을 지웁니다.</t>
+  </si>
+  <si>
+    <t>Eccentric_BombCenterMass.label</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bomb</t>
+  </si>
+  <si>
+    <t>Eccentric_BombCenterMass.deathMessage</t>
+  </si>
+  <si>
+    <t>{0} has died in an explosion.</t>
+  </si>
+  <si>
+    <t>폭탄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0}(이)가 폭발로 사망했습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eccentric_ShieldProjectorWide.label</t>
+  </si>
+  <si>
+    <t>Eccentric_ShieldProjectorWide.description</t>
+  </si>
+  <si>
+    <t>shield projector (wide-area)</t>
+  </si>
+  <si>
+    <t>A shield projector designed to be linked together to provide protection for a wide area.\n\nShield projectors do not need to be directly powered, but must be connected to a defense grid network with an active shield generator and shield capacitors to function. Intercepting incoming projectiles will also generate a great deal of heat which must be dissipated in heatsinks.\n\nThis wide-area variant can cover a much larger area but requires its own shield core.</t>
+  </si>
+  <si>
+    <t>쉴드 프로젝터 (광역)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>넓은 지역을 보호하기 위해 서로 연결하여 사용할 수 있도록 설계된 쉴드 프로젝터입니다.\n\n쉴드 프로젝터는 직접 전원을 공급할 필요는 없지만, 활성 쉴드 제너레이터와 쉴드 커패시터가 있는 방어망 네트워크에 연결해야 작동합니다. 또한 발사체를 요격하면 많은 양의 열이 발생하므로 방열판을 통해 열을 방출해야 합니다.\n\n이 광역 버전은 훨씬 더 넓은 영역을 보호할 수 있지만 자체 쉴드 코어가 필요합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eccentric_StandaloneShieldGenerator.comps.CompBurnoutBattery.inspectLabel</t>
+  </si>
+  <si>
+    <t>Power remaining: {0}/{1} ({2}%)</t>
+  </si>
+  <si>
+    <t>남은 전력: {0}/{1} ({2}%)</t>
+  </si>
+  <si>
+    <t>Eccentric_BluntExplosive.label</t>
+  </si>
+  <si>
+    <t>blunt</t>
+  </si>
+  <si>
+    <t>둔기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2525,24 +2783,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G177"/>
+  <dimension ref="A1:G206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="A200" sqref="A200"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="74.4140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.9140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="74.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.25" customWidth="1"/>
-    <col min="5" max="5" width="31.1640625" customWidth="1"/>
-    <col min="6" max="6" width="40.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.125" customWidth="1"/>
+    <col min="6" max="6" width="40.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2565,7 +2823,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>_xlfn.TEXTJOIN("+",,B2,C2)</f>
         <v>ConceptDef+EccentricDefenseGrid_TrackingMissiles.label</v>
@@ -2590,7 +2848,7 @@
         <v>추적 미사일</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:A66" si="0">_xlfn.TEXTJOIN("+",,B3,C3)</f>
         <v>ConceptDef+EccentricDefenseGrid_TrackingMissiles.helpText</v>
@@ -2615,7 +2873,7 @@
         <v>M48과 같은 능동 추적 대전차 미사일은 표적에 큰 피해를 입힐 수 있지만, 충분한 크기 또는 질량의 표적을 조준한 후에만 발사할 수 있습니다. 이 미사일은 최소 차체 크기가 1.5인 메카노이드와 전차 또는 최소 크기가 3.0인 유기 표적만 표적으로 삼을 수 있습니다.</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>DamageDef+Eccentric_BluntExplosive.deathMessage</v>
@@ -2640,7 +2898,7 @@
         <v>{0}(이)가 깔려 죽었습니다.</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>JobDef+EccentricDefenseGrid_ReloadMissileLauncher.reportString</v>
@@ -2665,7 +2923,7 @@
         <v>TargetB(을)를 TargetA에 장전합니다.</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>JobDef+EccentricDefenseGrid_UnloadMissileLauncher.reportString</v>
@@ -2687,7 +2945,7 @@
         <v>TargetA(을)를 장전 해제합니다.</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>JobDef+EccentricDefenseGrid_DesignateArtilleryTarget.reportString</v>
@@ -2709,7 +2967,7 @@
         <v>TargetB(을)를 사용하여 포격 목표를 지정 합니다.</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ResearchTabDef+Eccentric_Tech.label</v>
@@ -2731,7 +2989,7 @@
         <v>편심 기술</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ResearchProjectDef+Eccentric_DefenseGridNetwork.label</v>
@@ -2753,7 +3011,7 @@
         <v>네트워크 기반 방어</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ResearchProjectDef+Eccentric_DefenseGridNetwork.description</v>
@@ -2775,7 +3033,7 @@
         <v>네트워크로 연결된 방어 시스템을 위한 도관 구축의 기본을 연구합니다.</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ResearchProjectDef+Eccentric_DefenseGridArtillery.label</v>
@@ -2797,7 +3055,7 @@
         <v>네트워크 기반 포격</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ResearchProjectDef+Eccentric_DefenseGridArtillery.description</v>
@@ -2819,7 +3077,7 @@
         <v>근거리 유도 포격 지원을 위해 네트워크 미사일 발사대와 근접 센서 타워를 구축합니다.</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ResearchProjectDef+Eccentric_DefenseGridDesignators.label</v>
@@ -2841,7 +3099,7 @@
         <v>휴대용 표적지시기</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ResearchProjectDef+Eccentric_DefenseGridDesignators.description</v>
@@ -2863,7 +3121,7 @@
         <v>야전 레이저 지시기를 구축하여 미사일 포격의 사거리를 연장할 수 있습니다.</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ResearchProjectDef+Eccentric_DefenseGridShields.label</v>
@@ -2885,7 +3143,7 @@
         <v>네트워크 기반 쉴드</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ResearchProjectDef+Eccentric_DefenseGridShields.description</v>
@@ -2907,7 +3165,7 @@
         <v>네트워크 커패시터와 방열판을 사용한 광역 방어막을 구축합니다.</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ResearchProjectDef+Eccentric_DefenseGridShieldFabrication.label</v>
@@ -2929,7 +3187,7 @@
         <v>고 에너지 쉴드 코어</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ResearchProjectDef+Eccentric_DefenseGridShieldFabrication.description</v>
@@ -2951,7 +3209,7 @@
         <v>나노 조립기의 고 에너지 쉴드 코어 제작 기능을 잠금 해제합니다.</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingCategoryDef+EccentricApparel.label</v>
@@ -2973,7 +3231,7 @@
         <v>편심</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingCategoryDef+EccentricApparelUtility.label</v>
@@ -2995,7 +3253,7 @@
         <v>다용도구</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_ArtillerySensorTower.label</v>
@@ -3017,7 +3275,7 @@
         <v>근접 센서 타워</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_ArtillerySensorTower.description</v>
@@ -3039,7 +3297,7 @@
         <v>방어망 네트워크에 연결하면 유도탄을 원격으로 조준할 수 있는 정교한 센서 제품입니다. 연결된 네트워크의 미사일 런처는 중앙 콘솔에서 센서 타워 범위 내에 있는 표적을 향해 직접 발사할 수 있습니다.</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_ArtilleryVerticalMissileLauncher.label</v>
@@ -3061,7 +3319,7 @@
         <v>수직 미사일 런처</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_ArtilleryVerticalMissileLauncher.description</v>
@@ -3083,7 +3341,7 @@
         <v>군용 우주선에 사용되는 유닛을 기반으로 한 소형 수직 미사일 런처로, 원격으로 발사할 수 있으며 다양한 네트워크 장치에서 단말기 유도를 받을 수 있습니다. 엔진이 점화되기 전에 미사일을 발사하는 소프트 발사 시스템을 사용하여 발사기의 손상을 최소화하고 신속하게 재장전할 수 있습니다.</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_ShieldGenerator.label</v>
@@ -3105,7 +3363,7 @@
         <v>쉴드 제너레이터</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_ShieldGenerator.description</v>
@@ -3127,7 +3385,7 @@
         <v>연결된 프로젝터와 함께 작동하도록 설계된 군용 중앙 집중식 쉴드 발생 장치입니다.\n\n이 장치는 자체적으로 발사체를 요격할 수 없으며, 방어망 네트워크를 통해 쉴드 프로젝터와 쉴드 커패시터에 연결해야 합니다. 또한 발사체를 요격하면 많은 양의 열이 발생하므로 방열판을 통해 열을 방출해야 합니다.</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_ShieldProjector.label</v>
@@ -3149,7 +3407,7 @@
         <v>쉴드 프로젝터</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_ShieldProjector.description</v>
@@ -3171,7 +3429,7 @@
         <v>넓은 지역을 보호하기 위해 서로 연결하여 사용할 수 있도록 설계된 쉴드 프로젝터입니다.\n\n쉴드 프로젝터는 직접 전원을 공급할 필요는 없지만, 활성 쉴드 제너레이터와 쉴드 커패시터가 있는 방어망 네트워크에 연결해야 작동합니다. 또한 발사체를 요격하면 많은 양의 열이 발생하므로 방열판을 통해 열을 방출해야 합니다.</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_ShieldCapacitor.label</v>
@@ -3193,7 +3451,7 @@
         <v>쉴드 커패시터</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_ShieldCapacitor.description</v>
@@ -3215,7 +3473,7 @@
         <v>네트워크 쉴드 제너레이터에 전원을 공급하는 데 사용되는 고 에너지 커패시터입니다.\n\n충전하려면 전원에 직접 연결해야 하며, 전원이 공급되지 않으면 빠르게 방전됩니다.</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_ShieldHeatsink.label</v>
@@ -3237,7 +3495,7 @@
         <v>쉴드 방열판</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_ShieldHeatsink.description</v>
@@ -3259,7 +3517,7 @@
         <v>네트워크로 연결된 쉴드 제너레이터의 열을 방출하는 데 사용되는 대용량 방열판입니다.\n\n열을 받으려면 방어망 도관을 통해 쉴드 제너레이터에 연결해야 합니다.</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_StandaloneShieldGenerator.label</v>
@@ -3281,7 +3539,7 @@
         <v>배치형 쉴드 제너레이터</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_StandaloneShieldGenerator.description</v>
@@ -3303,7 +3561,7 @@
         <v>날아오는 발사체와 폭발물을 막을 수 있는 소형 쉴드 제너레이터입니다. 내부 전원이 제한되어 있으며 잠시 후 전원이 차단됩니다.</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_DefenseConduit.label</v>
@@ -3325,7 +3583,7 @@
         <v>방어망 도관</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_DefenseConduit.description</v>
@@ -3347,7 +3605,7 @@
         <v>군용 쉴드와 무기 시스템을 연결하는 데 사용되는 고 에너지 전력 링크와 냉각수 파이프라인이 포함된 정교한 도관입니다.\n\n벽이나 다른 건물 아래에 설치할 수 있습니다.</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_DefenseConduitUnderground.label</v>
@@ -3369,7 +3627,7 @@
         <v>지하 방어망 도관</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_DefenseConduitUnderground.description</v>
@@ -3391,7 +3649,7 @@
         <v>군용 쉴드와 무기 시스템을 연결하는 데 사용되는 고 에너지 전력 링크와 냉각수 파이프라인이 포함된 정교한 도관입니다.\n\n이 도관은 지하에 매설되기 때문에 건설에 더 많은 작업과 자재가 필요하지만, 도관이 손상되지 않도록 보호하고 주변을 덜 어수선하게 만듭니다.</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_DefenseGridConsole.label</v>
@@ -3413,7 +3671,7 @@
         <v>방어망 콘솔</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_DefenseGridConsole.description</v>
@@ -3435,7 +3693,7 @@
         <v>연결된 방어망 네트워크를 직접 제어할 수 있는 콘솔입니다. 원격으로 포격 지정을 하려면 콘솔에 사람이 있어야 합니다.</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_DefenseTurretController.label</v>
@@ -3457,7 +3715,7 @@
         <v>원격 포탑 컨트롤러</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_DefenseTurretController.description</v>
@@ -3479,7 +3737,7 @@
         <v>방어망 콘솔을 통해 유인 포탑을 원격으로 제어할 수 있는 인터페이스입니다. 한 명의 정착민이 하나의 콘솔에서 네트워크에 연결된 모든 유인 포탑을 제어할 수 있습니다.</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_HighEnergyShieldCore.label</v>
@@ -3501,7 +3759,7 @@
         <v>고 에너지 쉴드 코어</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+Eccentric_HighEnergyShieldCore.description</v>
@@ -3523,7 +3781,7 @@
         <v>광역 방어망에 필수적인 구성 요소입니다.\n\n이 복잡한 장치는 나노 규모의 정밀 생산 시설에서만 제작할 수 있기 때문에 변방계에서는 극히 드뭅니다.</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M36PGM.label</v>
@@ -3545,7 +3803,7 @@
         <v>M36 PGM (고폭탄)</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M36PGM.labelShort</v>
@@ -3567,7 +3825,7 @@
         <v>M36 HE</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M36PGM.description</v>
@@ -3589,7 +3847,7 @@
         <v>폭발력이 높은 탄두를 장착한 정밀 유도 단거리 지대지 미사일입니다.\n\n군용 우주선의 수직 미사일 런처에 장착할 수 있도록 설계되었으며, 발사 시 유도 고정 장치가 필요합니다.</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M38PGM.label</v>
@@ -3611,7 +3869,7 @@
         <v>M38 PGM (소이탄)</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M38PGM.labelShort</v>
@@ -3633,7 +3891,7 @@
         <v>M38 소이탄</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M38PGM.description</v>
@@ -3655,7 +3913,7 @@
         <v>휘발성 소이탄이 장착된 정밀 유도 단거리 지대지 미사일입니다.\n\n군용 우주선의 수직 미사일 런처에 장착할 수 있도록 설계되었으며, 발사 시 유도 고정 장치가 필요합니다.</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M39PGM.label</v>
@@ -3677,7 +3935,7 @@
         <v>M39 PGM (EMP탄)</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M39PGM.labelShort</v>
@@ -3699,7 +3957,7 @@
         <v>M39 EMP</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M39PGM.description</v>
@@ -3721,7 +3979,7 @@
         <v>전자기 펄스 탄두를 장착한 정밀 유도 단거리 지대지 미사일입니다.\n\n군용 우주선의 수직 미사일 런처에 장착할 수 있도록 설계되었으며, 발사 시 유도 고정 장치가 필요합니다.</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M48PGM.label</v>
@@ -3743,7 +4001,7 @@
         <v>M48 PGM (대전차 고폭탄)</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M48PGM.labelShort</v>
@@ -3765,7 +4023,7 @@
         <v>M48 HEAT</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M48PGM.description</v>
@@ -3787,7 +4045,7 @@
         <v>고폭탄 탄두를 장착한 정밀 유도 단거리 대전차 미사일입니다. 충분한 질량의 표적을 능동적으로 추적할 수 있지만 폭발 반경이 매우 작습니다.\n\n군용 우주선의 수직 미사일 런처에 장착할 수 있도록 설계되었으며, 발사 시 유도 고정 장치가 필요합니다.</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M56PGM.label</v>
@@ -3809,7 +4067,7 @@
         <v>M56 PGM (번아웃 쉴드탄)</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M56PGM.labelShort</v>
@@ -3831,7 +4089,7 @@
         <v>M56 쉴드</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M56PGM.description</v>
@@ -3853,7 +4111,7 @@
         <v>번아웃 쉴드 탄두가 장착된 정밀 유도 단거리 미사일입니다. 충돌 시 광역 보호막을 투사하는 임시 제너레이터를 배치하여 집중 포격을 받는 지상군을 지원하도록 설계되었습니다.\n\n군용 우주선의 수직 미사일 런처에 장착할 수 있도록 설계되었으며, 발사 시 유도 고정 장치가 필요합니다.</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M61PGM.label</v>
@@ -3875,7 +4133,7 @@
         <v>M61 PGM (반물질탄)</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M61PGM.labelShort</v>
@@ -3897,7 +4155,7 @@
         <v>M61 반물질</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Ordnance_M61PGM.description</v>
@@ -3919,7 +4177,7 @@
         <v>반물질 탄두를 장착한 정밀 유도 단거리 지대지 미사일입니다.\n\n군용 우주선의 수직 미사일 런처에 장착할 수 있도록 설계되었으며, 발사 시 유도 고정 장치가 필요합니다.</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M36PGM.label</v>
@@ -3941,7 +4199,7 @@
         <v>M36 정밀 유도 미사일</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M36PGM.modExtensions.0.stages.0.label</v>
@@ -3963,7 +4221,7 @@
         <v>사출</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M36PGM.modExtensions.0.stages.1.label</v>
@@ -3985,7 +4243,7 @@
         <v>추적</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="str">
         <f t="shared" si="0"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M38PGM.label</v>
@@ -4007,7 +4265,7 @@
         <v>M38 정밀 유도 미사일</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="str">
         <f t="shared" ref="A67:A130" si="1">_xlfn.TEXTJOIN("+",,B67,C67)</f>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M38PGM.modExtensions.0.stages.0.label</v>
@@ -4029,7 +4287,7 @@
         <v>사출</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M38PGM.modExtensions.0.stages.1.label</v>
@@ -4051,7 +4309,7 @@
         <v>추적</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M39PGM.label</v>
@@ -4073,7 +4331,7 @@
         <v>M39 정밀 유도 미사일</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M39PGM.modExtensions.0.stages.0.label</v>
@@ -4095,7 +4353,7 @@
         <v>사출</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M39PGM.modExtensions.0.stages.1.label</v>
@@ -4117,7 +4375,7 @@
         <v>추적</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M48PGM.label</v>
@@ -4139,7 +4397,7 @@
         <v>M48 정밀 유도 미사일</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M48PGM.modExtensions.0.stages.0.label</v>
@@ -4161,7 +4419,7 @@
         <v>사출</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M48PGM.modExtensions.0.stages.1.label</v>
@@ -4183,7 +4441,7 @@
         <v>추적</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M56PGM.label</v>
@@ -4205,7 +4463,7 @@
         <v>M56 정밀 유도 미사일</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M56PGM.modExtensions.0.stages.0.label</v>
@@ -4227,7 +4485,7 @@
         <v>사출</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M56PGM.modExtensions.0.stages.1.label</v>
@@ -4249,7 +4507,7 @@
         <v>추적</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M61PGM.label</v>
@@ -4271,7 +4529,7 @@
         <v>M61 정밀 유도 미사일</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M61PGM.modExtensions.0.stages.0.label</v>
@@ -4293,7 +4551,7 @@
         <v>사출</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ThingDef+EccentricDefenseGrid_Projectile_M61PGM.modExtensions.0.stages.1.label</v>
@@ -4315,7 +4573,7 @@
         <v>추적</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ThingDef+Eccentric_ArtilleryDesignator.label</v>
@@ -4337,7 +4595,7 @@
         <v>원격 포격 지시기</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ThingDef+Eccentric_ArtilleryDesignator.description</v>
@@ -4359,7 +4617,7 @@
         <v>지역 네트워크 방어망에서 포격을 지시하는 데 사용되는 소형 레이저 지시기입니다.</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="str">
         <f t="shared" si="1"/>
         <v>ThingDef+Eccentric_ArtilleryDesignator.comps.2.verb.label</v>
@@ -4381,7 +4639,7 @@
         <v>목표 지정</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="str">
         <f t="shared" si="1"/>
         <v>RecipeDef+Eccentric_MakeHighEnergyShieldCore.label</v>
@@ -4403,7 +4661,7 @@
         <v>고 에너지 쉴드 코어 제작</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="str">
         <f t="shared" si="1"/>
         <v>RecipeDef+Eccentric_MakeHighEnergyShieldCore.description</v>
@@ -4425,7 +4683,7 @@
         <v>고 에너지 쉴드 코어를 제작합니다.</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="str">
         <f t="shared" si="1"/>
         <v>RecipeDef+Eccentric_MakeHighEnergyShieldCore.jobString</v>
@@ -4447,7 +4705,7 @@
         <v>고 에너지 쉴드 코어 제작 중...</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WorkGiverDef+EccentricDefenseGrid_ReloadMissileLaunchers.label</v>
@@ -4469,7 +4727,7 @@
         <v>targetB(을)를 targetA에 장전</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WorkGiverDef+EccentricDefenseGrid_ReloadMissileLaunchers.verb</v>
@@ -4491,7 +4749,7 @@
         <v>장전</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WorkGiverDef+EccentricDefenseGrid_ReloadMissileLaunchers.gerund</v>
@@ -4513,7 +4771,7 @@
         <v>장전</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WorkGiverDef+EccentricDefenseGrid_UnloadMissileLaunchers.label</v>
@@ -4535,7 +4793,7 @@
         <v>targetA에서 탄약 장전 해제</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WorkGiverDef+EccentricDefenseGrid_UnloadMissileLaunchers.verb</v>
@@ -4557,7 +4815,7 @@
         <v>해제</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="str">
         <f t="shared" si="1"/>
         <v>WorkGiverDef+EccentricDefenseGrid_UnloadMissileLaunchers.gerund</v>
@@ -4579,7 +4837,7 @@
         <v>해제</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_LauncherDefaultName</v>
@@ -4601,7 +4859,7 @@
         <v>런처 {0}</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_LauncherRename</v>
@@ -4623,7 +4881,7 @@
         <v>이름 변경</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_LauncherRenameDesc</v>
@@ -4645,7 +4903,7 @@
         <v>이 런처의 라벨을 설정하거나 변경합니다.</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_LauncherRenamed</v>
@@ -4667,7 +4925,7 @@
         <v>런처 이름 설정 완료 : {0}</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_OrdnanceTabName</v>
@@ -4689,7 +4947,7 @@
         <v>무기</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_OrdnanceTabSlot</v>
@@ -4711,7 +4969,7 @@
         <v>슬롯 {0}</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_OrdnanceTabSlotEmpty</v>
@@ -4733,7 +4991,7 @@
         <v>(비어 있음)</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_OrdnanceTabAllSlots</v>
@@ -4755,7 +5013,7 @@
         <v>모든 슬롯</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_OrdnanceCount</v>
@@ -4777,7 +5035,7 @@
         <v>{0} ({1})</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_OrdnanceSelect</v>
@@ -4799,7 +5057,7 @@
         <v>(무기 선택)</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_OrdnanceUnload</v>
@@ -4821,7 +5079,7 @@
         <v>(무기 장전 해제)</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_OrdnanceAutoReload</v>
@@ -4843,7 +5101,7 @@
         <v>자동 재장전</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_OrdnanceReady</v>
@@ -4865,7 +5123,7 @@
         <v>발사 준비 완료</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_OrdnanceInactive</v>
@@ -4887,7 +5145,7 @@
         <v>비활성</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_OrdnanceStartingUp</v>
@@ -4909,7 +5167,7 @@
         <v>초기화 중... {0}초</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_OrdnanceOnCooldown</v>
@@ -4931,7 +5189,7 @@
         <v>재사용 대기 중... {0}초</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_ConfigMissingOrdnance</v>
@@ -4953,7 +5211,7 @@
         <v>OrdnanceDef {0}에 정의된 무기 속성이 없습니다.</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_ConfigMissingProjectile</v>
@@ -4975,7 +5233,7 @@
         <v>OrdnanceDef {0}의 무기 속성에 정의된 발사체가 없습니다.</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignateArtillery</v>
@@ -4997,7 +5255,7 @@
         <v>포격 지정</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignateArtilleryDesc</v>
@@ -5019,7 +5277,7 @@
         <v>지역 방어망 무기의 포격 대상을 지정합니다.\n\n마우스 오른쪽 버튼을 클릭하여 무기 유형을 선택합니다.</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignatorNotDraftedDesc</v>
@@ -5041,7 +5299,7 @@
         <v>사용하려면 소집되어야 합니다.</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignatorNotConnectedDesc</v>
@@ -5063,7 +5321,7 @@
         <v>연결할 지역 방어망을 찾을 수 없습니다.</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignatorNoOrdnanceDesc</v>
@@ -5085,7 +5343,7 @@
         <v>지역 방어망에 장전된 무기가 없습니다.</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignatorNoPawnDesc</v>
@@ -5107,7 +5365,7 @@
         <v>유인 콘솔 또는 현장 지시기 없이 포격을 지시할 수 없습니다.</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignatorErrorAntiTank</v>
@@ -5129,7 +5387,7 @@
         <v>대전차 무기는 충분한 크기 또는 밀도의 표적에만 고정할 수 있습니다.</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignatorErrorSensorRange</v>
@@ -5151,7 +5409,7 @@
         <v>목표물이 센서 타워 범위 밖에 있습니다.</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignatorCannotConnect</v>
@@ -5173,7 +5431,7 @@
         <v>오류 : 방어망 네트워크에 연결할 수 없습니다. 다시 시도하세요.</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignatorInvalidOrdnance</v>
@@ -5195,7 +5453,7 @@
         <v>오류 : 선택한 무기 유형이 잘못되었습니다.</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignatorEmptyOrdnance</v>
@@ -5217,7 +5475,7 @@
         <v>오류 : 선택한 무기 유형이 비어 있습니다.</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignatorOrdnanceUnavailable</v>
@@ -5239,7 +5497,7 @@
         <v>오류 : 선택한 무기 유형을 사용할 수 없습니다.</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignatorInvalidCaster</v>
@@ -5261,7 +5519,7 @@
         <v>오류 : 잘못된 폰이 대상을 지정하려고 했습니다.</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignatorCooldownActive</v>
@@ -5283,7 +5541,7 @@
         <v>오류 : 선택한 런처가 재사용 대기 중입니다.</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignatorNoneAvailable</v>
@@ -5305,7 +5563,7 @@
         <v>오류 : 런처를 발사할 수 없습니다.</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_NetworkNoOrdnanceDesc</v>
@@ -5327,7 +5585,7 @@
         <v>선택한 방어망에 장전된 무기가 없습니다.</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignationModeSingle</v>
@@ -5349,7 +5607,7 @@
         <v>단일</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignationModeSingleDesc</v>
@@ -5371,7 +5629,7 @@
         <v>사용 가능한 가장 가까운 런처에서 선택한 유형의 무기 한 발을 발사합니다.</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignationModeCluster</v>
@@ -5393,7 +5651,7 @@
         <v>클러스터</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Keyed+EccentricDefenseGrid_DesignationModeClusterDesc</v>
@@ -5415,9 +5673,9 @@
         <v>선택한 런처에서 모든 무기를 발사합니다.</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="str">
-        <f t="shared" ref="A131:A177" si="2">_xlfn.TEXTJOIN("+",,B131,C131)</f>
+        <f t="shared" ref="A131:A194" si="2">_xlfn.TEXTJOIN("+",,B131,C131)</f>
         <v>Keyed+EccentricDefenseGrid_DesignationModeVolley</v>
       </c>
       <c r="B131" s="1" t="s">
@@ -5437,7 +5695,7 @@
         <v>일제 포격</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_DesignationModeVolleyDesc</v>
@@ -5459,7 +5717,7 @@
         <v>사용 가능한 모든 런처에서 선택한 유형의 무기를 발사합니다.</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_CapacitorInspect</v>
@@ -5481,7 +5739,7 @@
         <v>쉴드 커패시터: {0}/{1} ({2}%)</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_HeatsinkInspect</v>
@@ -5503,7 +5761,7 @@
         <v>열: {0}/{1} ({2}%, {3})</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_GeneratorShutdown</v>
@@ -5525,7 +5783,7 @@
         <v>전력이 부족하여 {0}(이)가 꺼졌습니다!</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_GeneratorOverload</v>
@@ -5547,7 +5805,7 @@
         <v>열 과부하로 인해 {0}(이)가 꺼졌습니다!</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_PlaceConduitExists</v>
@@ -5569,7 +5827,7 @@
         <v>여기에 도관을 배치할 수 없습니다. 도관 또는 도관 청사진이 이미 존재합니다.</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_TurretNotConnected</v>
@@ -5591,7 +5849,7 @@
         <v>포탑에 연결되어 있지 않음</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_TurretConnectedToUnmanned</v>
@@ -5613,7 +5871,7 @@
         <v>다음에 연결됨: {0} (무인)</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_TurretConnectedToManned</v>
@@ -5635,7 +5893,7 @@
         <v>다음에 연결됨: {0} (유인)</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_DesignatorDeconstructConduit</v>
@@ -5657,7 +5915,7 @@
         <v>도관 해체</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_DesignatorDeconstructConduitDesc</v>
@@ -5679,7 +5937,7 @@
         <v>방어 네트워크 도관을 해체하고 일부 자원을 회수합니다.</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ModName</v>
@@ -5701,7 +5959,7 @@
         <v>- Eccentric Tech - Defense Grid -</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShowProjectorEffects</v>
@@ -5723,7 +5981,7 @@
         <v>프로젝터 효과 표시</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShowProjectorEffectsDesc</v>
@@ -5745,7 +6003,7 @@
         <v>활성된 쉴드 프로젝터의 시각 효과를 표시합니다.</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShowInterceptionEffects</v>
@@ -5767,7 +6025,7 @@
         <v>차단 효과 표시</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShowInterceptionEffectsDesc</v>
@@ -5789,7 +6047,7 @@
         <v>쉴드가 발사체를 차단할 때 시각 효과를 표시합니다.</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShowInterceptionGrid</v>
@@ -5811,7 +6069,7 @@
         <v>차단 격자 표시</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShowInterceptionGridDesc</v>
@@ -5833,7 +6091,7 @@
         <v>방어망 네트워크로 보호되는 맵의 영역 위에 오버레이를 표시합니다.</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShowDefenseGridStatus</v>
@@ -5855,7 +6113,7 @@
         <v>방어망 상태 창 표시</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShowDefenseGridStatusDesc</v>
@@ -5877,7 +6135,7 @@
         <v>방어망 상태 창을 표시합니다.</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_Reset</v>
@@ -5899,7 +6157,7 @@
         <v>초기화</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ResetStatusWindowPosition</v>
@@ -5921,7 +6179,7 @@
         <v>HUD 위치 초기화</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ResetStatusWindowPositionDesc</v>
@@ -5943,7 +6201,7 @@
         <v>방어망 HUD의 위치를 화면 중앙으로 초기화합니다. 도달할 수 없게 된 경우에 사용합니다.</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShieldUnmanned</v>
@@ -5965,7 +6223,7 @@
         <v>방어 네트워크 콘솔이 유인 상태이거나 호환되는 AI가 연결된 경우에만 재구성할 수 있습니다.</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShieldInterceptDirect</v>
@@ -5987,7 +6245,7 @@
         <v>직사 발사체 차단</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShieldInterceptDirectDesc</v>
@@ -6009,7 +6267,7 @@
         <v>화살, 총알, 수류탄, 대전차 로켓과 같은 직사 발사체를 차단합니다.</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShieldInterceptOverhead</v>
@@ -6031,7 +6289,7 @@
         <v>곡사 발사체 차단</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShieldInterceptOverheadDesc</v>
@@ -6053,7 +6311,7 @@
         <v>박격포탄, 포탄, 포격 로켓과 같은 곡사 발사체를 차단합니다.</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShieldInterceptExplosive</v>
@@ -6075,7 +6333,7 @@
         <v>폭발성 발사체 차단</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShieldInterceptExplosiveDesc</v>
@@ -6097,7 +6355,7 @@
         <v>수류탄, 로켓, 소이탄과 같은 폭발성 발사체를 차단합니다.</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShieldInterceptNonExplosive</v>
@@ -6119,7 +6377,7 @@
         <v>비폭발성 발사체 차단</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShieldInterceptNonExplosiveDesc</v>
@@ -6141,7 +6399,7 @@
         <v>화살, 총알, 파편, 기타 운동 탄환과 같은 비폭발성 발사체를 차단합니다.</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShieldInterceptEnergyThreshold</v>
@@ -6163,7 +6421,7 @@
         <v>최소 에너지 ({0}%)</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShieldInterceptEnergyThresholdDesc</v>
@@ -6185,7 +6443,7 @@
         <v>이 제너레이터가 발사체를 차단할 최소 에너지 보유량을 설정합니다. 이 임계값 미만이면 이 제너레이터는 발사체를 통과시킵니다.</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShieldInterceptEnergyThresholdLabel</v>
@@ -6207,7 +6465,7 @@
         <v>최소 에너지 : {0}%</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_ShieldInterceptToggle</v>
@@ -6229,7 +6487,7 @@
         <v>모든 제너레이터를 활성화 또는 비활성화하려면 클릭합니다.</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_StatusNoNetworks</v>
@@ -6251,7 +6509,7 @@
         <v>범위 내에 네트워크가 없습니다...</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_StatusAmount</v>
@@ -6273,7 +6531,7 @@
         <v>{0} / {1}</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_StatusEnergyTotal</v>
@@ -6295,7 +6553,7 @@
         <v>전체 시스템 에너지</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_StatusEnergyCount</v>
@@ -6317,7 +6575,7 @@
         <v>커패시터: {0}</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_StatusEnergyDesc</v>
@@ -6339,7 +6597,7 @@
         <v>이 네트워크에서 사용할 수 있는 쉴드 에너지의 총량입니다. 발사체를 차단하면 에너지가 소모되며, 에너지가 모두 소모되면 쉴드가 붕괴됩니다.</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_StatusEnergyAction</v>
@@ -6361,7 +6619,7 @@
         <v>커패시터 격자를 표시하거나 숨기려면 클릭합니다.</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_StatusHeatTotal</v>
@@ -6383,7 +6641,7 @@
         <v>총 시스템 발열</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_StatusHeatCount</v>
@@ -6405,7 +6663,7 @@
         <v>방열판: {0}</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_StatusHeatDesc</v>
@@ -6427,7 +6685,7 @@
         <v>이 네트워크의 총 발열입니다. 발사체를 차단하면 열이 발생하고 시스템 열이 너무 높으면 제너레이터에 과부하가 걸려 시스템 열이 다시 내려갈 때까지 제너레이터가 작동하지 않을 수 있습니다.</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Keyed+EccentricDefenseGrid_StatusHeatAction</v>
@@ -6447,6 +6705,528 @@
       <c r="G177" t="str">
         <f>IFERROR(VLOOKUP(A177,Update!$C$2:$D$179,2,FALSE),"")</f>
         <v>방열판 격자를 표시하거나 숨기려면 클릭합니다.</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A178" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_ProjectorEffects</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C178" t="s">
+        <v>705</v>
+      </c>
+      <c r="D178" t="s">
+        <v>728</v>
+      </c>
+      <c r="E178" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A179" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_ProjectorEffectsDesc</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C179" t="s">
+        <v>706</v>
+      </c>
+      <c r="D179" t="s">
+        <v>729</v>
+      </c>
+      <c r="E179" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A180" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_ShowProjectorEffectsSelected</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C180" t="s">
+        <v>707</v>
+      </c>
+      <c r="D180" t="s">
+        <v>730</v>
+      </c>
+      <c r="E180" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A181" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_ShowProjectorEffectsSelectedDesc</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C181" t="s">
+        <v>708</v>
+      </c>
+      <c r="D181" t="s">
+        <v>731</v>
+      </c>
+      <c r="E181" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A182" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_ShowProjectorEffectsSelectedNetwork</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C182" t="s">
+        <v>709</v>
+      </c>
+      <c r="D182" t="s">
+        <v>732</v>
+      </c>
+      <c r="E182" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A183" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_ShowProjectorEffectsSelectedNetworkDesc</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C183" t="s">
+        <v>710</v>
+      </c>
+      <c r="D183" t="s">
+        <v>733</v>
+      </c>
+      <c r="E183" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A184" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_ShowProjectorEffectsDanger</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C184" t="s">
+        <v>711</v>
+      </c>
+      <c r="D184" t="s">
+        <v>734</v>
+      </c>
+      <c r="E184" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A185" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_ShowProjectorEffectsDangerDesc</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C185" t="s">
+        <v>712</v>
+      </c>
+      <c r="D185" t="s">
+        <v>735</v>
+      </c>
+      <c r="E185" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A186" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_ShieldRadiusLabel</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C186" t="s">
+        <v>713</v>
+      </c>
+      <c r="D186" t="s">
+        <v>736</v>
+      </c>
+      <c r="E186" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A187" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_ShieldRadiusDesc</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C187" t="s">
+        <v>714</v>
+      </c>
+      <c r="D187" t="s">
+        <v>737</v>
+      </c>
+      <c r="E187" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A188" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_Color</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C188" t="s">
+        <v>715</v>
+      </c>
+      <c r="D188" t="s">
+        <v>738</v>
+      </c>
+      <c r="E188" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A189" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_ColorDesc</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C189" t="s">
+        <v>716</v>
+      </c>
+      <c r="D189" t="s">
+        <v>739</v>
+      </c>
+      <c r="E189" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A190" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_ColorDefault</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C190" t="s">
+        <v>717</v>
+      </c>
+      <c r="D190" t="s">
+        <v>740</v>
+      </c>
+      <c r="E190" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A191" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_ColorRedLabel</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C191" t="s">
+        <v>718</v>
+      </c>
+      <c r="D191" t="s">
+        <v>741</v>
+      </c>
+      <c r="E191" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A192" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_ColorGreenLabel</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C192" t="s">
+        <v>719</v>
+      </c>
+      <c r="D192" t="s">
+        <v>742</v>
+      </c>
+      <c r="E192" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A193" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_ColorBlueLabel</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C193" t="s">
+        <v>720</v>
+      </c>
+      <c r="D193" t="s">
+        <v>743</v>
+      </c>
+      <c r="E193" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A194" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Keyed+EccentricDefenseGrid_ColorAlphaLabel</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C194" t="s">
+        <v>721</v>
+      </c>
+      <c r="D194" t="s">
+        <v>744</v>
+      </c>
+      <c r="E194" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A195" s="1" t="str">
+        <f t="shared" ref="A195:A206" si="3">_xlfn.TEXTJOIN("+",,B195,C195)</f>
+        <v>Keyed+EccentricDefenseGrid_ColorCopy</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C195" t="s">
+        <v>722</v>
+      </c>
+      <c r="D195" t="s">
+        <v>745</v>
+      </c>
+      <c r="E195" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A196" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Keyed+EccentricDefenseGrid_ColorCopyDesc</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C196" t="s">
+        <v>723</v>
+      </c>
+      <c r="D196" t="s">
+        <v>746</v>
+      </c>
+      <c r="E196" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A197" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Keyed+EccentricDefenseGrid_ColorPaste</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C197" t="s">
+        <v>724</v>
+      </c>
+      <c r="D197" t="s">
+        <v>747</v>
+      </c>
+      <c r="E197" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A198" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Keyed+EccentricDefenseGrid_ColorPasteDesc</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C198" t="s">
+        <v>725</v>
+      </c>
+      <c r="D198" t="s">
+        <v>748</v>
+      </c>
+      <c r="E198" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A199" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Keyed+EccentricDefenseGrid_ColorClear</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C199" t="s">
+        <v>726</v>
+      </c>
+      <c r="D199" t="s">
+        <v>749</v>
+      </c>
+      <c r="E199" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A200" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Keyed+EccentricDefenseGrid_ColorClearDesc</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C200" t="s">
+        <v>727</v>
+      </c>
+      <c r="D200" t="s">
+        <v>750</v>
+      </c>
+      <c r="E200" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A201" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>DamageDef+Eccentric_BombCenterMass.label</v>
+      </c>
+      <c r="B201" t="s">
+        <v>16</v>
+      </c>
+      <c r="C201" t="s">
+        <v>770</v>
+      </c>
+      <c r="D201" t="s">
+        <v>771</v>
+      </c>
+      <c r="E201" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A202" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>DamageDef+Eccentric_BombCenterMass.deathMessage</v>
+      </c>
+      <c r="B202" t="s">
+        <v>16</v>
+      </c>
+      <c r="C202" t="s">
+        <v>772</v>
+      </c>
+      <c r="D202" t="s">
+        <v>773</v>
+      </c>
+      <c r="E202" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A203" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>DamageDef+Eccentric_BluntExplosive.label</v>
+      </c>
+      <c r="B203" t="s">
+        <v>16</v>
+      </c>
+      <c r="C203" t="s">
+        <v>785</v>
+      </c>
+      <c r="D203" t="s">
+        <v>786</v>
+      </c>
+      <c r="E203" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A204" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>ThingDef+Eccentric_ShieldProjectorWide.label</v>
+      </c>
+      <c r="B204" t="s">
+        <v>74</v>
+      </c>
+      <c r="C204" t="s">
+        <v>776</v>
+      </c>
+      <c r="D204" t="s">
+        <v>778</v>
+      </c>
+      <c r="E204" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A205" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>ThingDef+Eccentric_ShieldProjectorWide.description</v>
+      </c>
+      <c r="B205" t="s">
+        <v>74</v>
+      </c>
+      <c r="C205" t="s">
+        <v>777</v>
+      </c>
+      <c r="D205" t="s">
+        <v>779</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A206" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>ThingDef+Eccentric_StandaloneShieldGenerator.comps.CompBurnoutBattery.inspectLabel</v>
+      </c>
+      <c r="B206" t="s">
+        <v>74</v>
+      </c>
+      <c r="C206" t="s">
+        <v>782</v>
+      </c>
+      <c r="D206" t="s">
+        <v>783</v>
+      </c>
+      <c r="E206" t="s">
+        <v>784</v>
       </c>
     </row>
   </sheetData>
@@ -6459,19 +7239,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDB8B93-80B9-4DEE-AF69-B146A1488D41}">
   <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A145" workbookViewId="0">
       <selection activeCell="I168" sqref="I168"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="79.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="79.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.9140625" customWidth="1"/>
+    <col min="1" max="1" width="79.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>699</v>
       </c>
@@ -6482,7 +7262,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>280</v>
       </c>
@@ -6498,7 +7278,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>284</v>
       </c>
@@ -6514,7 +7294,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>287</v>
       </c>
@@ -6530,7 +7310,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>290</v>
       </c>
@@ -6546,7 +7326,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>293</v>
       </c>
@@ -6562,7 +7342,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>296</v>
       </c>
@@ -6578,7 +7358,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>299</v>
       </c>
@@ -6594,7 +7374,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>302</v>
       </c>
@@ -6610,7 +7390,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>305</v>
       </c>
@@ -6626,7 +7406,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>308</v>
       </c>
@@ -6642,7 +7422,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>311</v>
       </c>
@@ -6658,7 +7438,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>314</v>
       </c>
@@ -6674,7 +7454,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>317</v>
       </c>
@@ -6690,7 +7470,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>320</v>
       </c>
@@ -6706,7 +7486,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>323</v>
       </c>
@@ -6722,7 +7502,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>326</v>
       </c>
@@ -6738,7 +7518,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>329</v>
       </c>
@@ -6754,7 +7534,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>332</v>
       </c>
@@ -6770,7 +7550,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>335</v>
       </c>
@@ -6786,7 +7566,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>338</v>
       </c>
@@ -6802,7 +7582,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>341</v>
       </c>
@@ -6818,7 +7598,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>344</v>
       </c>
@@ -6834,7 +7614,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>347</v>
       </c>
@@ -6850,7 +7630,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>350</v>
       </c>
@@ -6866,7 +7646,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>353</v>
       </c>
@@ -6882,7 +7662,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>356</v>
       </c>
@@ -6898,7 +7678,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>359</v>
       </c>
@@ -6914,7 +7694,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>362</v>
       </c>
@@ -6930,7 +7710,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>365</v>
       </c>
@@ -6946,7 +7726,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>368</v>
       </c>
@@ -6962,7 +7742,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>371</v>
       </c>
@@ -6978,7 +7758,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>374</v>
       </c>
@@ -6994,7 +7774,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>377</v>
       </c>
@@ -7010,7 +7790,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>425</v>
       </c>
@@ -7026,7 +7806,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>428</v>
       </c>
@@ -7042,7 +7822,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>380</v>
       </c>
@@ -7058,7 +7838,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>383</v>
       </c>
@@ -7074,7 +7854,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>386</v>
       </c>
@@ -7090,7 +7870,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>389</v>
       </c>
@@ -7106,7 +7886,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>392</v>
       </c>
@@ -7122,7 +7902,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>395</v>
       </c>
@@ -7138,7 +7918,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>398</v>
       </c>
@@ -7154,7 +7934,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>401</v>
       </c>
@@ -7170,7 +7950,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>404</v>
       </c>
@@ -7186,7 +7966,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>407</v>
       </c>
@@ -7202,7 +7982,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>410</v>
       </c>
@@ -7218,7 +7998,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>413</v>
       </c>
@@ -7234,7 +8014,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>416</v>
       </c>
@@ -7250,7 +8030,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>419</v>
       </c>
@@ -7266,7 +8046,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>422</v>
       </c>
@@ -7282,7 +8062,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>431</v>
       </c>
@@ -7298,7 +8078,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>434</v>
       </c>
@@ -7314,7 +8094,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>437</v>
       </c>
@@ -7330,7 +8110,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>440</v>
       </c>
@@ -7346,7 +8126,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>443</v>
       </c>
@@ -7362,7 +8142,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>446</v>
       </c>
@@ -7378,7 +8158,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>449</v>
       </c>
@@ -7394,7 +8174,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>452</v>
       </c>
@@ -7410,7 +8190,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>455</v>
       </c>
@@ -7426,7 +8206,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>458</v>
       </c>
@@ -7442,7 +8222,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>461</v>
       </c>
@@ -7458,7 +8238,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>464</v>
       </c>
@@ -7474,7 +8254,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>467</v>
       </c>
@@ -7490,7 +8270,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>470</v>
       </c>
@@ -7506,7 +8286,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>473</v>
       </c>
@@ -7522,7 +8302,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>476</v>
       </c>
@@ -7538,7 +8318,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>479</v>
       </c>
@@ -7554,7 +8334,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>482</v>
       </c>
@@ -7570,7 +8350,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>485</v>
       </c>
@@ -7586,7 +8366,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>488</v>
       </c>
@@ -7602,7 +8382,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>491</v>
       </c>
@@ -7618,7 +8398,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>494</v>
       </c>
@@ -7634,7 +8414,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>497</v>
       </c>
@@ -7650,7 +8430,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>500</v>
       </c>
@@ -7666,7 +8446,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>503</v>
       </c>
@@ -7682,7 +8462,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>506</v>
       </c>
@@ -7698,7 +8478,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>509</v>
       </c>
@@ -7714,7 +8494,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>512</v>
       </c>
@@ -7730,7 +8510,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>515</v>
       </c>
@@ -7746,7 +8526,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>518</v>
       </c>
@@ -7762,7 +8542,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>521</v>
       </c>
@@ -7778,7 +8558,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>524</v>
       </c>
@@ -7794,7 +8574,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>527</v>
       </c>
@@ -7810,7 +8590,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>530</v>
       </c>
@@ -7826,7 +8606,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>533</v>
       </c>
@@ -7842,7 +8622,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>6</v>
       </c>
@@ -7858,7 +8638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>11</v>
       </c>
@@ -7874,7 +8654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>15</v>
       </c>
@@ -7890,7 +8670,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>622</v>
       </c>
@@ -7910,7 +8690,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>20</v>
       </c>
@@ -7926,7 +8706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>25</v>
       </c>
@@ -7942,7 +8722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>28</v>
       </c>
@@ -7958,7 +8738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>251</v>
       </c>
@@ -7974,7 +8754,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>255</v>
       </c>
@@ -7990,7 +8770,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>258</v>
       </c>
@@ -8006,7 +8786,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>35</v>
       </c>
@@ -8022,7 +8802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>39</v>
       </c>
@@ -8038,7 +8818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>42</v>
       </c>
@@ -8054,7 +8834,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>45</v>
       </c>
@@ -8070,7 +8850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>48</v>
       </c>
@@ -8086,7 +8866,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>51</v>
       </c>
@@ -8102,7 +8882,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>54</v>
       </c>
@@ -8118,7 +8898,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>57</v>
       </c>
@@ -8134,7 +8914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>60</v>
       </c>
@@ -8150,7 +8930,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>63</v>
       </c>
@@ -8166,7 +8946,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>31</v>
       </c>
@@ -8182,7 +8962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>66</v>
       </c>
@@ -8198,7 +8978,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>70</v>
       </c>
@@ -8214,7 +8994,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>73</v>
       </c>
@@ -8230,7 +9010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>77</v>
       </c>
@@ -8246,7 +9026,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>80</v>
       </c>
@@ -8262,7 +9042,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>83</v>
       </c>
@@ -8278,7 +9058,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>86</v>
       </c>
@@ -8294,7 +9074,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>89</v>
       </c>
@@ -8310,7 +9090,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>92</v>
       </c>
@@ -8326,7 +9106,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>95</v>
       </c>
@@ -8342,7 +9122,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>98</v>
       </c>
@@ -8358,7 +9138,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>101</v>
       </c>
@@ -8374,7 +9154,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>104</v>
       </c>
@@ -8390,7 +9170,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>107</v>
       </c>
@@ -8406,7 +9186,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>110</v>
       </c>
@@ -8422,7 +9202,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>113</v>
       </c>
@@ -8438,7 +9218,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>702</v>
       </c>
@@ -8454,7 +9234,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>116</v>
       </c>
@@ -8470,7 +9250,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>119</v>
       </c>
@@ -8486,7 +9266,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>122</v>
       </c>
@@ -8502,7 +9282,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>125</v>
       </c>
@@ -8518,7 +9298,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -8534,7 +9314,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>131</v>
       </c>
@@ -8550,7 +9330,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>134</v>
       </c>
@@ -8566,7 +9346,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>137</v>
       </c>
@@ -8582,7 +9362,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>140</v>
       </c>
@@ -8598,7 +9378,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>143</v>
       </c>
@@ -8614,7 +9394,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>146</v>
       </c>
@@ -8630,7 +9410,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>149</v>
       </c>
@@ -8646,7 +9426,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>152</v>
       </c>
@@ -8662,7 +9442,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>155</v>
       </c>
@@ -8678,7 +9458,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>158</v>
       </c>
@@ -8694,7 +9474,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>161</v>
       </c>
@@ -8710,7 +9490,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>164</v>
       </c>
@@ -8726,7 +9506,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>167</v>
       </c>
@@ -8742,7 +9522,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>170</v>
       </c>
@@ -8758,7 +9538,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>173</v>
       </c>
@@ -8774,7 +9554,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>176</v>
       </c>
@@ -8790,7 +9570,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>179</v>
       </c>
@@ -8806,7 +9586,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>182</v>
       </c>
@@ -8822,7 +9602,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>185</v>
       </c>
@@ -8838,7 +9618,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>188</v>
       </c>
@@ -8854,7 +9634,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>191</v>
       </c>
@@ -8870,7 +9650,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>194</v>
       </c>
@@ -8886,7 +9666,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>197</v>
       </c>
@@ -8902,7 +9682,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>200</v>
       </c>
@@ -8918,7 +9698,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>203</v>
       </c>
@@ -8934,7 +9714,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>206</v>
       </c>
@@ -8950,7 +9730,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>209</v>
       </c>
@@ -8966,7 +9746,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>212</v>
       </c>
@@ -8982,7 +9762,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>214</v>
       </c>
@@ -8998,7 +9778,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>216</v>
       </c>
@@ -9014,7 +9794,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>219</v>
       </c>
@@ -9030,7 +9810,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>221</v>
       </c>
@@ -9046,7 +9826,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>223</v>
       </c>
@@ -9062,7 +9842,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>226</v>
       </c>
@@ -9078,7 +9858,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>228</v>
       </c>
@@ -9094,7 +9874,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>230</v>
       </c>
@@ -9110,7 +9890,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>233</v>
       </c>
@@ -9126,7 +9906,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>235</v>
       </c>
@@ -9142,7 +9922,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>237</v>
       </c>
@@ -9158,7 +9938,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>240</v>
       </c>
@@ -9174,7 +9954,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>242</v>
       </c>
@@ -9190,7 +9970,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>244</v>
       </c>
@@ -9206,7 +9986,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>247</v>
       </c>
@@ -9222,7 +10002,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>692</v>
       </c>
@@ -9241,7 +10021,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>261</v>
       </c>
@@ -9257,7 +10037,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>265</v>
       </c>
@@ -9273,7 +10053,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>268</v>
       </c>
@@ -9289,7 +10069,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>271</v>
       </c>
@@ -9305,7 +10085,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>274</v>
       </c>
@@ -9321,7 +10101,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>277</v>
       </c>

</xml_diff>